<commit_message>
added additional Private Buyer ID for Yahoo tab
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/asoh-flask-deploy/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/PROD/prodplatformsapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E9F79CB-1418-A946-AD5F-0FCF9761A541}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB2173B-612D-844A-91A3-1D4497F8630F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39140" yWindow="3040" windowWidth="31860" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1580" yWindow="980" windowWidth="31860" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adform" sheetId="6" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="93">
   <si>
     <t>Segment ID</t>
   </si>
@@ -390,6 +390,16 @@
   </si>
   <si>
     <t>1589</t>
+  </si>
+  <si>
+    <t>Private Client ID</t>
+  </si>
+  <si>
+    <t>Optional
+(Separated by |)</t>
+  </si>
+  <si>
+    <t>1234|4567</t>
   </si>
 </sst>
 </file>
@@ -1793,7 +1803,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A046AC4F-D72D-9C40-94C8-967158865EC4}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -2072,19 +2082,20 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="77.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -2094,14 +2105,17 @@
       <c r="C1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="F1" s="13" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6" ht="34">
       <c r="A2" s="7" t="s">
         <v>5</v>
       </c>
@@ -2111,14 +2125,17 @@
       <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="18" t="s">
-        <v>6</v>
+      <c r="D2" s="9" t="s">
+        <v>91</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>1111</v>
       </c>
@@ -2129,7 +2146,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>2222</v>
       </c>
@@ -2138,6 +2155,9 @@
       </c>
       <c r="C4" t="s">
         <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Adobe AdCloud to uploadtemplate
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -8,25 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/PROD/prodplatformsapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB2173B-612D-844A-91A3-1D4497F8630F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F653D278-E639-904F-A118-825FA8830DAA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="980" windowWidth="31860" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8580" yWindow="1640" windowWidth="15620" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adform" sheetId="6" r:id="rId1"/>
     <sheet name="Adobe AAM" sheetId="5" r:id="rId2"/>
-    <sheet name="AppNexus" sheetId="3" r:id="rId3"/>
-    <sheet name="MediaMath" sheetId="8" r:id="rId4"/>
-    <sheet name="TTD" sheetId="1" r:id="rId5"/>
-    <sheet name="Yahoo" sheetId="4" r:id="rId6"/>
-    <sheet name="All Report Platforms" sheetId="7" r:id="rId7"/>
+    <sheet name="Adobe AdCloud" sheetId="9" r:id="rId3"/>
+    <sheet name="AppNexus" sheetId="3" r:id="rId4"/>
+    <sheet name="MediaMath" sheetId="8" r:id="rId5"/>
+    <sheet name="TTD" sheetId="1" r:id="rId6"/>
+    <sheet name="Yahoo" sheetId="4" r:id="rId7"/>
+    <sheet name="All Report Platforms" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="179021"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="98">
   <si>
     <t>Segment ID</t>
   </si>
@@ -400,6 +401,27 @@
   </si>
   <si>
     <t>1234|4567</t>
+  </si>
+  <si>
+    <t>Lifetime</t>
+  </si>
+  <si>
+    <t>Add: Not Required
+Edit: Required
+Query: Required</t>
+  </si>
+  <si>
+    <t>Add: Required
+Edit: Required
+Query: Not Required</t>
+  </si>
+  <si>
+    <t>Add: Not Required
+Edit: Required
+Query: Not Required</t>
+  </si>
+  <si>
+    <t>Test Segment 1</t>
   </si>
 </sst>
 </file>
@@ -1473,7 +1495,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -1612,6 +1634,85 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{689799C4-08DD-4348-87B9-856D4611FF5E}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="51">
+      <c r="A2" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>12345</v>
+      </c>
+      <c r="B3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0.75</v>
+      </c>
+      <c r="F3">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M4"/>
   <sheetViews>
@@ -1799,7 +1900,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A046AC4F-D72D-9C40-94C8-967158865EC4}">
   <dimension ref="A1:H7"/>
   <sheetViews>
@@ -1961,7 +2062,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
@@ -2080,11 +2181,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -2165,7 +2266,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ACD0D70-707D-6848-808A-BFBD2B8DA8BA}">
   <dimension ref="A1:B3"/>
   <sheetViews>

</xml_diff>

<commit_message>
add and edit functions for adobe adcloud
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/PROD/prodplatformsapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F653D278-E639-904F-A118-825FA8830DAA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8E1C1C-D3CB-974D-9C2E-944A1719E928}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8580" yWindow="1640" windowWidth="15620" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6040" yWindow="1640" windowWidth="24320" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adform" sheetId="6" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="101">
   <si>
     <t>Segment ID</t>
   </si>
@@ -406,22 +406,27 @@
     <t>Lifetime</t>
   </si>
   <si>
-    <t>Add: Not Required
-Edit: Required
-Query: Required</t>
-  </si>
-  <si>
-    <t>Add: Required
-Edit: Required
-Query: Not Required</t>
-  </si>
-  <si>
-    <t>Add: Not Required
-Edit: Required
-Query: Not Required</t>
-  </si>
-  <si>
     <t>Test Segment 1</t>
+  </si>
+  <si>
+    <t>Add Custom: Required
+Edit Custom: Required</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>455399-e1ecec9c</t>
+  </si>
+  <si>
+    <t>Eyeota Segment ID</t>
+  </si>
+  <si>
+    <t>Add Custom: Not Required
+Edit Custom: Required</t>
+  </si>
+  <si>
+    <t>AdCloud Segment ID</t>
   </si>
 </sst>
 </file>
@@ -774,7 +779,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -917,6 +922,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -963,7 +979,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1021,6 +1037,9 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1635,41 +1654,50 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{689799C4-08DD-4348-87B9-856D4611FF5E}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="51">
-      <c r="A2" s="12" t="s">
-        <v>94</v>
+      <c r="H1" s="26" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="34">
+      <c r="A2" s="10" t="s">
+        <v>95</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>95</v>
@@ -1677,33 +1705,42 @@
       <c r="C2" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="D2" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3">
+      <c r="D2" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3">
         <v>12345</v>
       </c>
-      <c r="B3" t="s">
-        <v>97</v>
-      </c>
       <c r="C3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" t="s">
         <v>56</v>
       </c>
-      <c r="D3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3">
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3">
         <v>0.75</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated UploadTemplate and fixed appnexus data usage report for deleted segment ids
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/PROD/prodplatformsapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8E1C1C-D3CB-974D-9C2E-944A1719E928}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95EC91C1-E880-394B-9BFF-6D05DCF48CE2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6040" yWindow="1640" windowWidth="24320" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6040" yWindow="1640" windowWidth="24320" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adform" sheetId="6" r:id="rId1"/>
@@ -1513,8 +1513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3:M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -1640,10 +1640,10 @@
       <c r="H3">
         <v>0</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <v>1</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1656,7 +1656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{689799C4-08DD-4348-87B9-856D4611FF5E}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added Add custom segments and Edit custom segments function for TTD
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/PROD/prodplatformsapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95EC91C1-E880-394B-9BFF-6D05DCF48CE2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{75E499EA-76D1-454C-9F14-A282C0C0FD51}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6040" yWindow="1640" windowWidth="24320" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6040" yWindow="1640" windowWidth="24320" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adform" sheetId="6" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="96">
   <si>
     <t>Segment ID</t>
   </si>
@@ -50,24 +50,6 @@
     <t>Optional</t>
   </si>
   <si>
-    <t>Premium Range Purchasers</t>
-  </si>
-  <si>
-    <t>Users who prefer premium branded ranges over supermarket own brand</t>
-  </si>
-  <si>
-    <t>UK Kantar Media TGI &gt; Grocery Shopping &gt; Premium Range Purchasers</t>
-  </si>
-  <si>
-    <t>TV Channels Watched Live (Last 30 Days)</t>
-  </si>
-  <si>
-    <t>Not Buyable</t>
-  </si>
-  <si>
-    <t>Media &gt; TV And Film &gt; TV Channels Watched Live (Last 30 Days)</t>
-  </si>
-  <si>
     <t>Parent Segment ID</t>
   </si>
   <si>
@@ -108,9 +90,6 @@
   </si>
   <si>
     <t>Just random segment 2222</t>
-  </si>
-  <si>
-    <t>taxoapitest</t>
   </si>
   <si>
     <t>Data Source Name</t>
@@ -427,6 +406,12 @@
   </si>
   <si>
     <t>AdCloud Segment ID</t>
+  </si>
+  <si>
+    <t>ttdratetest_partnerID_rate</t>
+  </si>
+  <si>
+    <t>Test Segment 20190401003</t>
   </si>
 </sst>
 </file>
@@ -1420,57 +1405,57 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="68">
       <c r="A2" s="20" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1479,10 +1464,10 @@
         <v>20181130001</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1491,7 +1476,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="H3" s="3">
         <v>43405</v>
@@ -1513,7 +1498,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="L3" sqref="L3:M3"/>
     </sheetView>
   </sheetViews>
@@ -1538,104 +1523,104 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="119">
       <c r="A2" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="L2" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" s="12" t="s">
         <v>37</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="M2" s="12" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C3">
         <v>90</v>
       </c>
       <c r="D3" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="E3" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="F3" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="G3" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -1644,7 +1629,7 @@
         <v>1</v>
       </c>
       <c r="M3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1671,68 +1656,68 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" s="26" t="s">
         <v>93</v>
-      </c>
-      <c r="H1" s="26" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="34">
       <c r="A2" s="10" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B3">
         <v>12345</v>
       </c>
       <c r="C3" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
@@ -1776,81 +1761,81 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>20</v>
-      </c>
       <c r="G1" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>22</v>
-      </c>
       <c r="L1" s="13" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="M1" s="13" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="68" customHeight="1">
       <c r="A2" s="12" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="L2" s="14" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -1861,10 +1846,10 @@
         <v>-2018113011</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
@@ -1873,7 +1858,7 @@
         <v>129600</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H3" t="b">
         <v>1</v>
@@ -1899,10 +1884,10 @@
         <v>-2018113012</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
@@ -1911,7 +1896,7 @@
         <v>129600</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H4" t="b">
         <v>1</v>
@@ -1960,16 +1945,16 @@
         <v>1</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>2</v>
@@ -1997,10 +1982,10 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C3" s="23">
         <v>1</v>
@@ -2019,10 +2004,10 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -2039,10 +2024,10 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -2059,7 +2044,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -2076,10 +2061,10 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -2103,8 +2088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -2117,13 +2102,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>2</v>
@@ -2132,7 +2117,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H1" s="15" t="s">
         <v>4</v>
@@ -2166,52 +2151,23 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3">
-        <v>32048</v>
+        <v>20190401003</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>94</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3">
-        <v>3</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3" t="s">
-        <v>12</v>
+        <v>95</v>
+      </c>
+      <c r="D3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4">
-        <v>31804</v>
-      </c>
-      <c r="B4">
-        <v>31804</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-      <c r="G4" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="H4" t="s">
-        <v>9</v>
-      </c>
+      <c r="G4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2241,16 +2197,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="34">
@@ -2264,7 +2220,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>6</v>
@@ -2278,10 +2234,10 @@
         <v>1111</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2289,13 +2245,13 @@
         <v>2222</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -2315,18 +2271,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="13" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="68">
       <c r="A2" s="19" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2">

</xml_diff>

<commit_message>
added rates api functions for TTD
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/PROD/prodplatformsapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A98461-7345-164E-82E3-78EE70B9F54F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E402105-8723-1243-8808-8911031FD57F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6040" yWindow="1640" windowWidth="24320" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3200" yWindow="2040" windowWidth="29360" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adform" sheetId="6" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="111">
   <si>
     <t>Segment ID</t>
   </si>
@@ -435,6 +435,52 @@
   </si>
   <si>
     <t>In-Market</t>
+  </si>
+  <si>
+    <t>Brand</t>
+  </si>
+  <si>
+    <t>abc123</t>
+  </si>
+  <si>
+    <t>bombora</t>
+  </si>
+  <si>
+    <t>Seat ID</t>
+  </si>
+  <si>
+    <t>Batch ID</t>
+  </si>
+  <si>
+    <t>Add/Edit: Required
+Edit Rates: Required
+Retrieve Batch: Optional
+Retrieve Rates: Optional</t>
+  </si>
+  <si>
+    <t>Add/Edit: Required
+Edit Rates: Optional
+Retrieve Batch: Optional
+Retrieve Rates: Optional</t>
+  </si>
+  <si>
+    <t>Add/Edit: Required
+Edit Rates: Required
+Retrieve Batch: Optional
+Retrieve Rates: Required
+"bombora" or "eyeota" only</t>
+  </si>
+  <si>
+    <t>Add/Edit: Required
+Edit Rates: Required
+Retrieve Batch: Optional
+Retrieve Rates: Required</t>
+  </si>
+  <si>
+    <t>Add/Edit: Optional
+Edit Rates: Optional
+Retrieve Batch: Required
+Retrieve Rates: Optional</t>
   </si>
 </sst>
 </file>
@@ -987,7 +1033,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1024,7 +1070,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1050,6 +1095,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1454,7 +1505,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="68">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>51</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -1483,7 +1534,7 @@
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="20"/>
+      <c r="A3" s="19"/>
       <c r="B3">
         <v>20181130001</v>
       </c>
@@ -1510,8 +1561,8 @@
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1544,7 +1595,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -1588,7 +1639,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="136">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>90</v>
       </c>
       <c r="B2" s="10" t="s">
@@ -1707,7 +1758,7 @@
       <c r="G1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="24" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1769,7 +1820,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
@@ -2018,20 +2069,20 @@
       <c r="B3" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="22">
+      <c r="C3" s="21">
         <v>1</v>
       </c>
-      <c r="D3" s="22">
+      <c r="D3" s="21">
         <v>1</v>
       </c>
-      <c r="E3" s="22">
+      <c r="E3" s="21">
         <v>1</v>
       </c>
-      <c r="F3" s="23" t="b">
+      <c r="F3" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="G3" s="23"/>
-      <c r="H3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="21"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
@@ -2049,7 +2100,7 @@
       <c r="E4">
         <v>2</v>
       </c>
-      <c r="F4" s="23" t="b">
+      <c r="F4" s="22" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2069,7 +2120,7 @@
       <c r="E5">
         <v>3</v>
       </c>
-      <c r="F5" s="23" t="b">
+      <c r="F5" s="22" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2086,7 +2137,7 @@
       <c r="E6">
         <v>4</v>
       </c>
-      <c r="F6" s="24" t="b">
+      <c r="F6" s="23" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2106,7 +2157,7 @@
       <c r="E7">
         <v>5</v>
       </c>
-      <c r="F7" s="24" t="b">
+      <c r="F7" s="23" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2117,18 +2168,25 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="A10:H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="8" max="8" width="66.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.83203125" customWidth="1"/>
+    <col min="6" max="6" width="27.33203125" customWidth="1"/>
+    <col min="7" max="7" width="23.83203125" customWidth="1"/>
+    <col min="8" max="8" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="34">
+    <row r="1" spans="1:11" ht="17">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -2145,42 +2203,60 @@
         <v>2</v>
       </c>
       <c r="F1" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="J1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="14" t="s">
+      <c r="K1" s="14" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="16" t="s">
+    <row r="2" spans="1:11" ht="85">
+      <c r="A2" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="J2" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="K2" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>20190401003</v>
       </c>
@@ -2196,9 +2272,22 @@
       <c r="E3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="G4" s="1"/>
+      <c r="F3" t="s">
+        <v>103</v>
+      </c>
+      <c r="G3" t="s">
+        <v>102</v>
+      </c>
+      <c r="H3">
+        <v>1.25</v>
+      </c>
+      <c r="I3">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2253,10 +2342,10 @@
       <c r="D2" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="16" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2309,7 +2398,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="68">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>39</v>
       </c>
       <c r="B2" s="10" t="s">

</xml_diff>

<commit_message>
added delete segments function for adform
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/PROD/prodplatformsapp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/Local/localplatformsapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E402105-8723-1243-8808-8911031FD57F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8EBF91C-4C74-CC40-B74E-94761181F2EF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="2040" windowWidth="29360" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3200" yWindow="2040" windowWidth="29360" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adform" sheetId="6" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="112">
   <si>
     <t>Segment ID</t>
   </si>
@@ -234,18 +234,8 @@
     <t>Eyeota Segment Name</t>
   </si>
   <si>
-    <t>Add: Not required
-Edit: Required</t>
-  </si>
-  <si>
     <t>Add: Required
 Edit: Required</t>
-  </si>
-  <si>
-    <t>Add: Required
-Edit: Required
-Values: global, apac
-Defaulted to global</t>
   </si>
   <si>
     <t>Distribution</t>
@@ -481,6 +471,23 @@
 Edit Rates: Optional
 Retrieve Batch: Required
 Retrieve Rates: Optional</t>
+  </si>
+  <si>
+    <t>Add: Not required
+Edit: Required
+Delete: Required</t>
+  </si>
+  <si>
+    <t>Add: Required
+Edit: Required
+Delete: Not Required</t>
+  </si>
+  <si>
+    <t>Add: Required
+Edit: Required
+Delete: Not Required
+Values: global, apac
+Defaulted to global</t>
   </si>
 </sst>
 </file>
@@ -1459,18 +1466,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07DE401A-9862-6C4F-BF9F-D68D31DB6CEF}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" customWidth="1"/>
     <col min="4" max="4" width="18.33203125" customWidth="1"/>
-    <col min="5" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" customWidth="1"/>
+    <col min="6" max="7" width="19" customWidth="1"/>
     <col min="8" max="8" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1495,7 +1502,7 @@
         <v>42</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>37</v>
@@ -1504,27 +1511,27 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="68">
+    <row r="2" spans="1:9" ht="82" customHeight="1">
       <c r="A2" s="18" t="s">
-        <v>51</v>
+        <v>109</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>52</v>
+        <v>110</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>52</v>
+        <v>110</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>53</v>
+        <v>111</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>52</v>
+        <v>110</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>52</v>
+        <v>110</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>52</v>
+        <v>110</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>39</v>
@@ -1539,7 +1546,7 @@
         <v>20181130001</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D3" t="s">
         <v>44</v>
@@ -1551,7 +1558,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H3" s="3">
         <v>43405</v>
@@ -1617,7 +1624,7 @@
         <v>32</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>22</v>
@@ -1640,46 +1647,46 @@
     </row>
     <row r="2" spans="1:14" ht="136">
       <c r="A2" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="F2" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="E2" s="11" t="s">
+      <c r="H2" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="F2" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="G2" s="11" t="s">
+      <c r="I2" s="10" t="s">
         <v>93</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>95</v>
       </c>
       <c r="J2" s="11" t="s">
         <v>33</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L2" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="M2" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N2" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -1693,16 +1700,16 @@
         <v>90</v>
       </c>
       <c r="E3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1738,10 +1745,10 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -1750,53 +1757,53 @@
         <v>8</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>34</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H1" s="24" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="34">
       <c r="A2" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B3">
         <v>12345</v>
       </c>
       <c r="C3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D3" t="s">
         <v>45</v>
@@ -1864,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J1" s="12" t="s">
         <v>11</v>
@@ -1881,7 +1888,7 @@
     </row>
     <row r="2" spans="1:13" ht="68" customHeight="1">
       <c r="A2" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>26</v>
@@ -1928,7 +1935,7 @@
         <v>-2018113011</v>
       </c>
       <c r="C3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D3" t="s">
         <v>45</v>
@@ -1946,7 +1953,7 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J3">
         <v>4299</v>
@@ -1966,7 +1973,7 @@
         <v>-2018113012</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D4" t="s">
         <v>46</v>
@@ -1984,7 +1991,7 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J4">
         <v>4299</v>
@@ -2030,13 +2037,13 @@
         <v>9</v>
       </c>
       <c r="C1" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>65</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>67</v>
       </c>
       <c r="F1" s="12" t="s">
         <v>2</v>
@@ -2064,10 +2071,10 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C3" s="21">
         <v>1</v>
@@ -2086,10 +2093,10 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -2106,10 +2113,10 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -2126,7 +2133,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -2143,10 +2150,10 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -2170,7 +2177,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
@@ -2203,16 +2210,16 @@
         <v>2</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H1" s="14" t="s">
         <v>13</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J1" s="14" t="s">
         <v>3</v>
@@ -2223,31 +2230,31 @@
     </row>
     <row r="2" spans="1:11" ht="85">
       <c r="A2" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="G2" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="27" t="s">
-        <v>107</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>107</v>
-      </c>
-      <c r="E2" s="27" t="s">
-        <v>107</v>
-      </c>
-      <c r="F2" s="27" t="s">
+      <c r="H2" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="I2" s="27" t="s">
         <v>108</v>
-      </c>
-      <c r="G2" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="H2" s="27" t="s">
-        <v>106</v>
-      </c>
-      <c r="I2" s="27" t="s">
-        <v>110</v>
       </c>
       <c r="J2" s="28" t="s">
         <v>6</v>
@@ -2261,22 +2268,22 @@
         <v>20190401003</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H3">
         <v>1.25</v>
@@ -2320,7 +2327,7 @@
         <v>8</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E1" s="12" t="s">
         <v>49</v>
@@ -2340,7 +2347,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E2" s="16" t="s">
         <v>6</v>
@@ -2371,7 +2378,7 @@
         <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Price Rates for TTD to accommodate percent media
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/Local/localplatformsapp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/PROD/prodplatformsapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8EBF91C-4C74-CC40-B74E-94761181F2EF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81BCD870-A890-664B-AD77-46376FD2653E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="2040" windowWidth="29360" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3200" yWindow="2040" windowWidth="29360" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adform" sheetId="6" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="117">
   <si>
     <t>Segment ID</t>
   </si>
@@ -488,6 +488,25 @@
 Delete: Not Required
 Values: global, apac
 Defaulted to global</t>
+  </si>
+  <si>
+    <t>Price Type</t>
+  </si>
+  <si>
+    <t>Add/Edit: Required
+Edit Rates: Required
+Retrieve Batch: Optional
+Retrieve Rates: Optional
+Values: CPM or PercentOfMediaCost</t>
+  </si>
+  <si>
+    <t>PercentOfMediaCost</t>
+  </si>
+  <si>
+    <t>eyeota</t>
+  </si>
+  <si>
+    <t>Test Segment 20190401004</t>
   </si>
 </sst>
 </file>
@@ -1466,8 +1485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07DE401A-9862-6C4F-BF9F-D68D31DB6CEF}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:I2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2175,10 +2194,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -2189,11 +2208,12 @@
     <col min="6" max="6" width="27.33203125" customWidth="1"/>
     <col min="7" max="7" width="23.83203125" customWidth="1"/>
     <col min="8" max="8" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.6640625" customWidth="1"/>
+    <col min="9" max="9" width="21.5" customWidth="1"/>
+    <col min="10" max="10" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17">
+    <row r="1" spans="1:12" ht="17">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -2219,16 +2239,19 @@
         <v>13</v>
       </c>
       <c r="I1" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="J1" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="K1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="L1" s="14" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="85">
+    <row r="2" spans="1:12" ht="102">
       <c r="A2" s="27" t="s">
         <v>104</v>
       </c>
@@ -2254,16 +2277,19 @@
         <v>104</v>
       </c>
       <c r="I2" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="J2" s="27" t="s">
         <v>108</v>
-      </c>
-      <c r="J2" s="28" t="s">
-        <v>6</v>
       </c>
       <c r="K2" s="28" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="L2" s="28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3">
         <v>20190401003</v>
       </c>
@@ -2288,13 +2314,44 @@
       <c r="H3">
         <v>1.25</v>
       </c>
-      <c r="I3">
+      <c r="I3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3">
         <v>12345</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
+    <row r="4" spans="1:12">
+      <c r="A4">
+        <v>20190401004</v>
+      </c>
+      <c r="B4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G4" t="s">
+        <v>100</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>114</v>
+      </c>
+      <c r="J4">
+        <v>23456</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
added get uniques for AAM
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/PROD/prodplatformsapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81BCD870-A890-664B-AD77-46376FD2653E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9ABE0F-37D7-A344-BBED-E824829C7429}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="2040" windowWidth="29360" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3200" yWindow="2040" windowWidth="29360" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adform" sheetId="6" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="118">
   <si>
     <t>Segment ID</t>
   </si>
@@ -507,6 +507,11 @@
   </si>
   <si>
     <t>Test Segment 20190401004</t>
+  </si>
+  <si>
+    <t>Add: Required
+Edit: Required
+Get Uniques: Required</t>
   </si>
 </sst>
 </file>
@@ -1599,8 +1604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -1609,7 +1614,7 @@
     <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="14.6640625" customWidth="1"/>
-    <col min="6" max="6" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" customWidth="1"/>
     <col min="7" max="7" width="29.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.1640625" customWidth="1"/>
     <col min="9" max="9" width="26.1640625" bestFit="1" customWidth="1"/>
@@ -1681,7 +1686,7 @@
         <v>90</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>51</v>
+        <v>117</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>91</v>
@@ -2196,8 +2201,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C7:M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
separated requirement for Add and Edit segments for TTD Upload template
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/PROD/prodplatformsapp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/Local/localplatformsapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9ABE0F-37D7-A344-BBED-E824829C7429}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7563D9E6-2CF8-7A47-A152-4AC8468B917A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="2040" windowWidth="29360" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3200" yWindow="2040" windowWidth="29360" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adform" sheetId="6" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="119">
   <si>
     <t>Segment ID</t>
   </si>
@@ -442,37 +442,6 @@
     <t>Batch ID</t>
   </si>
   <si>
-    <t>Add/Edit: Required
-Edit Rates: Required
-Retrieve Batch: Optional
-Retrieve Rates: Optional</t>
-  </si>
-  <si>
-    <t>Add/Edit: Required
-Edit Rates: Optional
-Retrieve Batch: Optional
-Retrieve Rates: Optional</t>
-  </si>
-  <si>
-    <t>Add/Edit: Required
-Edit Rates: Required
-Retrieve Batch: Optional
-Retrieve Rates: Required
-"bombora" or "eyeota" only</t>
-  </si>
-  <si>
-    <t>Add/Edit: Required
-Edit Rates: Required
-Retrieve Batch: Optional
-Retrieve Rates: Required</t>
-  </si>
-  <si>
-    <t>Add/Edit: Optional
-Edit Rates: Optional
-Retrieve Batch: Required
-Retrieve Rates: Optional</t>
-  </si>
-  <si>
     <t>Add: Not required
 Edit: Required
 Delete: Required</t>
@@ -493,25 +462,69 @@
     <t>Price Type</t>
   </si>
   <si>
-    <t>Add/Edit: Required
+    <t>PercentOfMediaCost</t>
+  </si>
+  <si>
+    <t>eyeota</t>
+  </si>
+  <si>
+    <t>Test Segment 20190401004</t>
+  </si>
+  <si>
+    <t>Add: Required
+Edit: Required
+Get Uniques: Required</t>
+  </si>
+  <si>
+    <t>Add: Required
+Edit: Required
+Edit Rates: Required
+Retrieve Batch: Optional
+Retrieve Rates: Optional</t>
+  </si>
+  <si>
+    <t>Add: Required
+Edit: Required
+Edit Rates: Optional
+Retrieve Batch: Optional
+Retrieve Rates: Optional</t>
+  </si>
+  <si>
+    <t>Add: Required
+Edit: Not Required
+Edit Rates: Required
+Retrieve Batch: Optional
+Retrieve Rates: Required
+"bombora" or "eyeota" only</t>
+  </si>
+  <si>
+    <t>Add: Required
+Edit: Not Required
+Edit Rates: Required
+Retrieve Batch: Optional
+Retrieve Rates: Required</t>
+  </si>
+  <si>
+    <t>Add: Required
+Edit: Not Required
+Edit Rates: Required
+Retrieve Batch: Optional
+Retrieve Rates: Optional</t>
+  </si>
+  <si>
+    <t>Add: Required
+Edit: Not Required
 Edit Rates: Required
 Retrieve Batch: Optional
 Retrieve Rates: Optional
 Values: CPM or PercentOfMediaCost</t>
   </si>
   <si>
-    <t>PercentOfMediaCost</t>
-  </si>
-  <si>
-    <t>eyeota</t>
-  </si>
-  <si>
-    <t>Test Segment 20190401004</t>
-  </si>
-  <si>
-    <t>Add: Required
-Edit: Required
-Get Uniques: Required</t>
+    <t>Add: Not Required
+Edit: Not Required
+Edit Rates: Optional
+Retrieve Batch: Required
+Retrieve Rates: Optional</t>
   </si>
 </sst>
 </file>
@@ -1064,7 +1077,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1131,6 +1144,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1537,25 +1553,25 @@
     </row>
     <row r="2" spans="1:9" ht="82" customHeight="1">
       <c r="A2" s="18" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>39</v>
@@ -1604,7 +1620,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
@@ -1686,7 +1702,7 @@
         <v>90</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>91</v>
@@ -2201,8 +2217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C7:M8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -2244,7 +2260,7 @@
         <v>13</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="J1" s="14" t="s">
         <v>103</v>
@@ -2256,36 +2272,36 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="102">
+    <row r="2" spans="1:12" ht="119">
       <c r="A2" s="27" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="E2" s="27" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="F2" s="27" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="G2" s="27" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="H2" s="27" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="I2" s="27" t="s">
-        <v>113</v>
-      </c>
-      <c r="J2" s="27" t="s">
-        <v>108</v>
+        <v>117</v>
+      </c>
+      <c r="J2" s="29" t="s">
+        <v>118</v>
       </c>
       <c r="K2" s="28" t="s">
         <v>6</v>
@@ -2334,16 +2350,16 @@
         <v>86</v>
       </c>
       <c r="C4" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D4" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="G4" t="s">
         <v>100</v>
@@ -2352,7 +2368,7 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="J4">
         <v>23456</v>

</xml_diff>

<commit_message>
TTD Advertiser ID indicated as do not use
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/Local/localplatformsapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C361F1-26FD-2644-9190-EE37FDE87A8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC6453E9-D164-7242-B4B3-473BBEA61215}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3200" yWindow="2040" windowWidth="29360" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="122">
   <si>
     <t>Segment ID</t>
   </si>
@@ -436,9 +436,6 @@
     <t>bombora</t>
   </si>
   <si>
-    <t>Seat ID</t>
-  </si>
-  <si>
     <t>Batch ID</t>
   </si>
   <si>
@@ -481,13 +478,6 @@
 Edit Rates: Optional
 Retrieve Batch: Optional
 Retrieve Custom: Optional</t>
-  </si>
-  <si>
-    <t>Add: Required
-Edit: Not Required
-Edit Rates: Required
-Retrieve Batch: Optional
-Retrieve Custom: Required</t>
   </si>
   <si>
     <t>Add: Required
@@ -525,6 +515,25 @@
 Retrieve Batch: Optional
 Retrieve Custom: Optional
 "bombora" or "eyeota" only</t>
+  </si>
+  <si>
+    <t>Partner ID</t>
+  </si>
+  <si>
+    <t>Add: Optional
+Edit: Not Required
+Edit Rates: Optional
+Retrieve Batch: Optional
+Retrieve Custom: Required</t>
+  </si>
+  <si>
+    <t>Advertiser ID</t>
+  </si>
+  <si>
+    <t>def456</t>
+  </si>
+  <si>
+    <t>Do not use!!</t>
   </si>
 </sst>
 </file>
@@ -690,7 +699,7 @@
       <name val="Calibri (Body)_x0000_"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -873,6 +882,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1077,7 +1092,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1146,6 +1161,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1553,25 +1571,25 @@
     </row>
     <row r="2" spans="1:9" ht="82" customHeight="1">
       <c r="A2" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C2" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>106</v>
-      </c>
       <c r="E2" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>39</v>
@@ -1702,7 +1720,7 @@
         <v>90</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>91</v>
@@ -2215,10 +2233,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -2227,13 +2245,13 @@
     <col min="2" max="4" width="28.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.83203125" customWidth="1"/>
     <col min="6" max="6" width="27.33203125" customWidth="1"/>
-    <col min="7" max="8" width="23.83203125" customWidth="1"/>
-    <col min="9" max="9" width="24.1640625" customWidth="1"/>
-    <col min="10" max="10" width="24.6640625" customWidth="1"/>
-    <col min="12" max="12" width="16.6640625" customWidth="1"/>
+    <col min="7" max="9" width="23.83203125" customWidth="1"/>
+    <col min="10" max="10" width="24.1640625" customWidth="1"/>
+    <col min="11" max="11" width="24.6640625" customWidth="1"/>
+    <col min="13" max="13" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="17">
+    <row r="1" spans="1:13" ht="17">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -2253,63 +2271,69 @@
         <v>99</v>
       </c>
       <c r="G1" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="K1" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="H1" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="K1" s="14" t="s">
+      <c r="L1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="M1" s="14" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="119">
+    <row r="2" spans="1:13" ht="119">
       <c r="A2" s="27" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B2" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="H2" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="I2" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="C2" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="E2" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>118</v>
-      </c>
-      <c r="G2" s="27" t="s">
+      <c r="J2" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="H2" s="27" t="s">
+      <c r="K2" s="29" t="s">
         <v>114</v>
-      </c>
-      <c r="I2" s="27" t="s">
-        <v>115</v>
-      </c>
-      <c r="J2" s="29" t="s">
-        <v>116</v>
-      </c>
-      <c r="K2" s="28" t="s">
-        <v>6</v>
       </c>
       <c r="L2" s="28" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="M2" s="28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3">
         <v>20190401003</v>
       </c>
@@ -2331,17 +2355,20 @@
       <c r="G3" t="s">
         <v>100</v>
       </c>
-      <c r="H3">
+      <c r="H3" t="s">
+        <v>120</v>
+      </c>
+      <c r="I3">
         <v>1.25</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>34</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>12345</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:13">
       <c r="A4">
         <v>20190401004</v>
       </c>
@@ -2349,27 +2376,30 @@
         <v>86</v>
       </c>
       <c r="C4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G4" t="s">
         <v>100</v>
       </c>
-      <c r="H4">
+      <c r="H4" t="s">
+        <v>120</v>
+      </c>
+      <c r="I4">
         <v>1</v>
       </c>
-      <c r="I4" t="s">
-        <v>108</v>
-      </c>
-      <c r="J4">
+      <c r="J4" t="s">
+        <v>107</v>
+      </c>
+      <c r="K4">
         <v>23456</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed brand id for ttd
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/Local/localplatformsapp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/PROD/prodplatformsapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC6453E9-D164-7242-B4B3-473BBEA61215}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD10A92F-090F-5741-A09E-A49E4EFF80B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3200" yWindow="2040" windowWidth="29360" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -509,31 +509,31 @@
 Retrieve Custom: Required</t>
   </si>
   <si>
+    <t>Partner ID</t>
+  </si>
+  <si>
+    <t>Add: Optional
+Edit: Not Required
+Edit Rates: Optional
+Retrieve Batch: Optional
+Retrieve Custom: Required</t>
+  </si>
+  <si>
+    <t>Advertiser ID</t>
+  </si>
+  <si>
+    <t>def456</t>
+  </si>
+  <si>
+    <t>Do not use!!</t>
+  </si>
+  <si>
     <t>Add: Required
 Edit: Not Required
 Edit Rates: Required
 Retrieve Batch: Optional
 Retrieve Custom: Optional
-"bombora" or "eyeota" only</t>
-  </si>
-  <si>
-    <t>Partner ID</t>
-  </si>
-  <si>
-    <t>Add: Optional
-Edit: Not Required
-Edit Rates: Optional
-Retrieve Batch: Optional
-Retrieve Custom: Required</t>
-  </si>
-  <si>
-    <t>Advertiser ID</t>
-  </si>
-  <si>
-    <t>def456</t>
-  </si>
-  <si>
-    <t>Do not use!!</t>
+"bombora" or "eyeota" or fill in the Brand ID</t>
   </si>
 </sst>
 </file>
@@ -2236,7 +2236,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -2271,10 +2271,10 @@
         <v>99</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I1" s="14" t="s">
         <v>13</v>
@@ -2309,13 +2309,13 @@
         <v>111</v>
       </c>
       <c r="F2" s="27" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="G2" s="27" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H2" s="30" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I2" s="27" t="s">
         <v>112</v>
@@ -2356,7 +2356,7 @@
         <v>100</v>
       </c>
       <c r="H3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I3">
         <v>1.25</v>
@@ -2391,7 +2391,7 @@
         <v>100</v>
       </c>
       <c r="H4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I4">
         <v>1</v>

</xml_diff>

<commit_message>
changed fake partner id in uploadtemplate
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/PROD/prodplatformsapp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Data Ops/Heroku/PROD/prodplatformsapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD10A92F-090F-5741-A09E-A49E4EFF80B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E97A27B6-4DF8-E34B-A2B4-BD7AB6CA3415}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3200" yWindow="2040" windowWidth="29360" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -430,9 +430,6 @@
     <t>Brand</t>
   </si>
   <si>
-    <t>abc123</t>
-  </si>
-  <si>
     <t>bombora</t>
   </si>
   <si>
@@ -534,6 +531,9 @@
 Retrieve Batch: Optional
 Retrieve Custom: Optional
 "bombora" or "eyeota" or fill in the Brand ID</t>
+  </si>
+  <si>
+    <t>7s3xqae</t>
   </si>
 </sst>
 </file>
@@ -1571,25 +1571,25 @@
     </row>
     <row r="2" spans="1:9" ht="82" customHeight="1">
       <c r="A2" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C2" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>105</v>
-      </c>
       <c r="E2" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>39</v>
@@ -1720,7 +1720,7 @@
         <v>90</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>91</v>
@@ -2236,7 +2236,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -2271,19 +2271,19 @@
         <v>99</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I1" s="14" t="s">
         <v>13</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L1" s="14" t="s">
         <v>3</v>
@@ -2294,37 +2294,37 @@
     </row>
     <row r="2" spans="1:13" ht="119">
       <c r="A2" s="27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B2" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="H2" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="I2" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="C2" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="E2" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>121</v>
-      </c>
-      <c r="G2" s="27" t="s">
-        <v>117</v>
-      </c>
-      <c r="H2" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="I2" s="27" t="s">
+      <c r="J2" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="J2" s="27" t="s">
+      <c r="K2" s="29" t="s">
         <v>113</v>
-      </c>
-      <c r="K2" s="29" t="s">
-        <v>114</v>
       </c>
       <c r="L2" s="28" t="s">
         <v>6</v>
@@ -2350,13 +2350,13 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G3" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="H3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I3">
         <v>1.25</v>
@@ -2376,28 +2376,28 @@
         <v>86</v>
       </c>
       <c r="C4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G4" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="H4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I4">
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K4">
         <v>23456</v>

</xml_diff>